<commit_message>
adapted to new target
</commit_message>
<xml_diff>
--- a/data/DATAMODEL_ashrae.xlsx
+++ b/data/DATAMODEL_ashrae.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BCAD5B-D5FA-42E9-A2AB-424588B3DE1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ACF343-4DF4-4E66-A2D5-F82C80054DEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-119" yWindow="-119" windowWidth="28741" windowHeight="15677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>table</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>exclude</t>
+  </si>
+  <si>
+    <t>dayofyear</t>
   </si>
 </sst>
 </file>
@@ -611,24 +614,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="10.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="29.7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -671,7 +674,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -691,7 +694,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -711,7 +714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="29.7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -728,7 +731,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="29.7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -745,7 +748,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -759,7 +762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -776,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -790,7 +793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -807,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -824,47 +827,44 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="44.55" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -872,13 +872,19 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -886,16 +892,13 @@
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -903,13 +906,16 @@
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -917,16 +923,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -934,13 +937,16 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -948,13 +954,13 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -962,27 +968,27 @@
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -990,13 +996,13 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -1004,13 +1010,13 @@
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -1018,10 +1024,13 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1029,50 +1038,41 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1080,16 +1080,19 @@
         <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1097,13 +1100,16 @@
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1111,16 +1117,13 @@
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1128,37 +1131,54 @@
         <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29.7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G33" s="3"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G34" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1170,7 +1190,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1182,7 +1202,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>